<commit_message>
Update visual info excel, edit pipeline
</commit_message>
<xml_diff>
--- a/Visual information and models .xlsx
+++ b/Visual information and models .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21269\Desktop\Visual-Extraction-Leyton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E7241-A54D-4467-B5FD-30E41A35A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C47B20-A84F-475B-9F68-32B6678B138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="264" yWindow="828" windowWidth="21624" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Visual Information</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Links</t>
   </si>
   <si>
-    <t>Code snippet</t>
-  </si>
-  <si>
     <t>Tables</t>
   </si>
   <si>
@@ -169,13 +166,58 @@
   </si>
   <si>
     <t>passportPDF.py</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Code Snippets</t>
+  </si>
+  <si>
+    <t>Check version</t>
+  </si>
+  <si>
+    <t>PDF/Scanned Doc ?</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Focus on logos</t>
+  </si>
+  <si>
+    <t>Where is the info. Models of detection, models of recognition ?</t>
+  </si>
+  <si>
+    <t>Quality metric</t>
+  </si>
+  <si>
+    <t>Open Source ?</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Inference Time</t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>Add table to notion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +229,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,9 +268,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -232,6 +288,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4E384030-69EE-4E9E-99C0-63C2A1FDEA5A}" name="Table2" displayName="Table2" ref="D3:M15" totalsRowShown="0">
+  <autoFilter ref="D3:M15" xr:uid="{4E384030-69EE-4E9E-99C0-63C2A1FDEA5A}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{F84C20F6-6599-43EE-848C-AEB22B9C25C1}" name="Visual Information"/>
+    <tableColumn id="2" xr3:uid="{07A0B9BD-66B8-4B43-8F54-7EB536B2071B}" name="Models to use"/>
+    <tableColumn id="3" xr3:uid="{3722D258-B7B4-4821-A770-01F72AD405E6}" name="Links" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{C3556C0F-ED67-493C-8C4C-74CBE947AA28}" name="Code Snippets"/>
+    <tableColumn id="5" xr3:uid="{114E1883-E381-49B1-890F-C2D632828288}" name="Observations"/>
+    <tableColumn id="6" xr3:uid="{8AFE029A-B719-48DE-AF78-77EA6639EAD3}" name="PDF/Scanned Doc ?"/>
+    <tableColumn id="7" xr3:uid="{C9BE25FA-E3ED-4EA1-82CF-6B1B341E8D22}" name="Open Source ?"/>
+    <tableColumn id="8" xr3:uid="{735DBAB5-A0A1-4346-B91D-9181CEB26FA1}" name="Column1"/>
+    <tableColumn id="9" xr3:uid="{85A4E518-9329-414B-8E35-DBE6728ACE26}" name="Test"/>
+    <tableColumn id="10" xr3:uid="{5E304236-B683-4E1A-99FC-ED970801D76E}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,168 +572,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:G14"/>
+  <dimension ref="D3:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
     <col min="6" max="6" width="118.109375" customWidth="1"/>
     <col min="7" max="7" width="24.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G12" t="s">
         <v>35</v>
       </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
+      <c r="E13" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>40</v>
@@ -666,29 +766,61 @@
       <c r="G13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G15" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>47</v>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" xr:uid="{3A0140BF-D0B1-47C7-AC57-9BA5AADEE3DB}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{FF4E3C1A-830F-478E-B032-6860A366A01B}"/>
-    <hyperlink ref="F12" r:id="rId3" xr:uid="{877913A1-5EA7-404E-9FDB-E9ED05AC8396}"/>
-    <hyperlink ref="F14" r:id="rId4" xr:uid="{029E3734-93E1-4F56-8FEE-2835785C4116}"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{3A0140BF-D0B1-47C7-AC57-9BA5AADEE3DB}"/>
+    <hyperlink ref="F14" r:id="rId2" xr:uid="{FF4E3C1A-830F-478E-B032-6860A366A01B}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{877913A1-5EA7-404E-9FDB-E9ED05AC8396}"/>
+    <hyperlink ref="F15" r:id="rId4" xr:uid="{029E3734-93E1-4F56-8FEE-2835785C4116}"/>
+    <hyperlink ref="F4" r:id="rId5" location="example" xr:uid="{8E5A4E6F-AEBC-4872-941F-F668B3847739}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{64B6125E-5E55-425E-ABF9-E5E3A4FD77AC}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{A8453317-1D63-4DF4-ADCC-61E414ADF822}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{715BF0CA-492A-4273-82E8-AB6AA23FD3CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+  <tableParts count="1">
+    <tablePart r:id="rId10"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>